<commit_message>
Update BBT_TCs document with actual test results
</commit_message>
<xml_diff>
--- a/Docs/Lab02/Lab02_BBT_TCs_Form.xlsx
+++ b/Docs/Lab02/Lab02_BBT_TCs_Form.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28526"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7305370-B33B-4E6C-941F-7DDC9F8F7D08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{166A6D64-D547-4CB5-B5EC-E5195BC49337}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Statement" sheetId="1" r:id="rId1"/>
@@ -128,7 +128,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="123">
   <si>
     <t>VVSS, Info Romana, 2024-2025</t>
   </si>
@@ -426,9 +426,6 @@
     <t>Re-tested</t>
   </si>
   <si>
-    <t>not yet</t>
-  </si>
-  <si>
     <t>Chelaru Laurentiu</t>
   </si>
   <si>
@@ -751,6 +748,18 @@
   </si>
   <si>
     <t>TC15_BVA</t>
+  </si>
+  <si>
+    <t>not applicable</t>
+  </si>
+  <si>
+    <t>Payment type cannot be null</t>
+  </si>
+  <si>
+    <t>Payment amount cannot be negative</t>
+  </si>
+  <si>
+    <t>Table number must be between 1 and 8</t>
   </si>
 </sst>
 </file>
@@ -1434,7 +1443,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="136">
+  <cellXfs count="139">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1544,6 +1553,12 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1559,6 +1574,72 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1568,29 +1649,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1598,131 +1682,104 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1739,60 +1796,21 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2117,12 +2135,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="C1" s="50" t="s">
+      <c r="C1" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="52"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="58"/>
       <c r="H1" s="48" t="s">
         <v>1</v>
       </c>
@@ -2130,11 +2148,11 @@
       <c r="J1" s="48"/>
     </row>
     <row r="2" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="H2" s="53" t="s">
+      <c r="H2" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="53"/>
-      <c r="J2" s="53"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="59"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.3">
       <c r="H3" s="2"/>
@@ -2150,7 +2168,7 @@
         <v>5</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J4" s="2">
         <v>232</v>
@@ -2161,7 +2179,7 @@
         <v>6</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J5" s="2">
         <v>232</v>
@@ -2173,7 +2191,7 @@
         <v>7</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J6" s="2">
         <v>232</v>
@@ -2213,8 +2231,8 @@
       <c r="E13" s="1"/>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B14" s="128" t="s">
-        <v>66</v>
+      <c r="B14" s="49" t="s">
+        <v>65</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -2227,7 +2245,7 @@
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -2235,24 +2253,24 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
@@ -2315,21 +2333,21 @@
       <c r="N29" s="1"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B30" s="49" t="s">
+      <c r="B30" s="55" t="s">
         <v>18</v>
       </c>
-      <c r="C30" s="49"/>
-      <c r="D30" s="49"/>
-      <c r="E30" s="49"/>
-      <c r="F30" s="49"/>
-      <c r="G30" s="49"/>
-      <c r="H30" s="49"/>
-      <c r="I30" s="49"/>
-      <c r="J30" s="49"/>
-      <c r="K30" s="49"/>
-      <c r="L30" s="49"/>
-      <c r="M30" s="49"/>
-      <c r="N30" s="49"/>
+      <c r="C30" s="55"/>
+      <c r="D30" s="55"/>
+      <c r="E30" s="55"/>
+      <c r="F30" s="55"/>
+      <c r="G30" s="55"/>
+      <c r="H30" s="55"/>
+      <c r="I30" s="55"/>
+      <c r="J30" s="55"/>
+      <c r="K30" s="55"/>
+      <c r="L30" s="55"/>
+      <c r="M30" s="55"/>
+      <c r="N30" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2372,43 +2390,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="52"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="58"/>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B3" s="70" t="s">
-        <v>72</v>
-      </c>
-      <c r="C3" s="71"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="71"/>
-      <c r="G3" s="72"/>
+      <c r="B3" s="63" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="65"/>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B5" s="73" t="s">
+      <c r="B5" s="66" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="73"/>
-      <c r="D5" s="73"/>
-      <c r="E5" s="73"/>
-      <c r="G5" s="74" t="s">
+      <c r="C5" s="66"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="66"/>
+      <c r="G5" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="74"/>
-      <c r="I5" s="74"/>
-      <c r="J5" s="74"/>
-      <c r="K5" s="74"/>
-      <c r="L5" s="74"/>
-      <c r="M5" s="74"/>
-      <c r="N5" s="74"/>
-      <c r="O5" s="74"/>
-      <c r="P5" s="74"/>
-      <c r="Q5" s="74"/>
+      <c r="H5" s="67"/>
+      <c r="I5" s="67"/>
+      <c r="J5" s="67"/>
+      <c r="K5" s="67"/>
+      <c r="L5" s="67"/>
+      <c r="M5" s="67"/>
+      <c r="N5" s="67"/>
+      <c r="O5" s="67"/>
+      <c r="P5" s="67"/>
+      <c r="Q5" s="67"/>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B6" s="21" t="s">
@@ -2423,257 +2441,257 @@
       <c r="E6" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="75" t="s">
+      <c r="G6" s="68" t="s">
         <v>25</v>
       </c>
-      <c r="H6" s="61" t="s">
+      <c r="H6" s="78" t="s">
         <v>26</v>
       </c>
-      <c r="I6" s="59" t="s">
+      <c r="I6" s="76" t="s">
         <v>27</v>
       </c>
-      <c r="J6" s="64"/>
-      <c r="K6" s="64"/>
-      <c r="L6" s="64"/>
-      <c r="M6" s="64"/>
-      <c r="N6" s="64"/>
-      <c r="O6" s="60"/>
-      <c r="P6" s="63" t="s">
+      <c r="J6" s="81"/>
+      <c r="K6" s="81"/>
+      <c r="L6" s="81"/>
+      <c r="M6" s="81"/>
+      <c r="N6" s="81"/>
+      <c r="O6" s="77"/>
+      <c r="P6" s="80" t="s">
         <v>28</v>
       </c>
-      <c r="Q6" s="63"/>
+      <c r="Q6" s="80"/>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B7" s="4">
         <v>1</v>
       </c>
-      <c r="C7" s="67" t="s">
-        <v>73</v>
+      <c r="C7" s="60" t="s">
+        <v>72</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E7" s="4"/>
-      <c r="G7" s="76"/>
-      <c r="H7" s="62"/>
+      <c r="G7" s="69"/>
+      <c r="H7" s="79"/>
       <c r="I7" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="J7" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="J7" s="21" t="s">
+      <c r="K7" s="21" t="s">
         <v>85</v>
-      </c>
-      <c r="K7" s="21" t="s">
-        <v>86</v>
       </c>
       <c r="L7" s="21"/>
       <c r="M7" s="21"/>
-      <c r="N7" s="59"/>
-      <c r="O7" s="60"/>
-      <c r="P7" s="59" t="s">
+      <c r="N7" s="76"/>
+      <c r="O7" s="77"/>
+      <c r="P7" s="76" t="s">
         <v>29</v>
       </c>
-      <c r="Q7" s="60"/>
+      <c r="Q7" s="77"/>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B8" s="4">
         <v>2</v>
       </c>
-      <c r="C8" s="67"/>
+      <c r="C8" s="60"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G8" s="21">
         <v>1</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J8" s="32" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K8" s="32" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="L8" s="32"/>
       <c r="M8" s="32"/>
-      <c r="N8" s="79"/>
-      <c r="O8" s="80"/>
-      <c r="P8" s="79" t="s">
-        <v>88</v>
-      </c>
-      <c r="Q8" s="80"/>
+      <c r="N8" s="72"/>
+      <c r="O8" s="73"/>
+      <c r="P8" s="72" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q8" s="73"/>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B9" s="4">
         <v>3</v>
       </c>
-      <c r="C9" s="67" t="s">
-        <v>75</v>
+      <c r="C9" s="60" t="s">
+        <v>74</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E9" s="4"/>
       <c r="G9" s="21">
         <v>2</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="32"/>
       <c r="K9" s="32"/>
       <c r="L9" s="32"/>
       <c r="M9" s="32"/>
-      <c r="N9" s="79"/>
-      <c r="O9" s="80"/>
-      <c r="P9" s="79" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q9" s="80"/>
+      <c r="N9" s="72"/>
+      <c r="O9" s="73"/>
+      <c r="P9" s="72" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q9" s="73"/>
     </row>
     <row r="10" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B10" s="4">
         <v>4</v>
       </c>
-      <c r="C10" s="67"/>
+      <c r="C10" s="60"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G10" s="34">
         <v>3</v>
       </c>
-      <c r="H10" s="129" t="s">
-        <v>113</v>
+      <c r="H10" s="50" t="s">
+        <v>112</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J10" s="32" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K10" s="32" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="L10" s="32"/>
       <c r="M10" s="32"/>
-      <c r="N10" s="79"/>
-      <c r="O10" s="80"/>
-      <c r="P10" s="79" t="s">
-        <v>89</v>
-      </c>
-      <c r="Q10" s="80"/>
+      <c r="N10" s="72"/>
+      <c r="O10" s="73"/>
+      <c r="P10" s="72" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q10" s="73"/>
     </row>
     <row r="11" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="4">
         <v>5</v>
       </c>
-      <c r="C11" s="67" t="s">
-        <v>77</v>
+      <c r="C11" s="60" t="s">
+        <v>76</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E11" s="4"/>
       <c r="G11" s="34">
         <v>4</v>
       </c>
-      <c r="H11" s="130" t="s">
-        <v>93</v>
+      <c r="H11" s="51" t="s">
+        <v>92</v>
       </c>
       <c r="I11" s="12"/>
       <c r="J11" s="32"/>
       <c r="K11" s="32"/>
       <c r="L11" s="32"/>
       <c r="M11" s="32"/>
-      <c r="N11" s="79"/>
-      <c r="O11" s="80"/>
-      <c r="P11" s="79" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q11" s="80"/>
+      <c r="N11" s="72"/>
+      <c r="O11" s="73"/>
+      <c r="P11" s="72" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q11" s="73"/>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B12" s="4">
         <v>6</v>
       </c>
-      <c r="C12" s="67"/>
+      <c r="C12" s="60"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G12" s="11">
         <v>5</v>
       </c>
-      <c r="H12" s="130" t="s">
-        <v>94</v>
+      <c r="H12" s="51" t="s">
+        <v>93</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J12" s="32" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K12" s="32" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="L12" s="32"/>
       <c r="M12" s="32"/>
       <c r="N12" s="32"/>
       <c r="O12" s="32"/>
-      <c r="P12" s="79" t="s">
-        <v>89</v>
-      </c>
-      <c r="Q12" s="80"/>
+      <c r="P12" s="72" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q12" s="73"/>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B13" s="4">
         <v>7</v>
       </c>
-      <c r="C13" s="68" t="s">
-        <v>79</v>
+      <c r="C13" s="61" t="s">
+        <v>78</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E13" s="4"/>
       <c r="G13" s="11">
         <v>6</v>
       </c>
-      <c r="H13" s="130" t="s">
-        <v>95</v>
+      <c r="H13" s="51" t="s">
+        <v>94</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J13" s="32" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K13" s="32" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="L13" s="32"/>
       <c r="M13" s="32"/>
-      <c r="N13" s="79"/>
-      <c r="O13" s="80"/>
-      <c r="P13" s="79" t="s">
-        <v>89</v>
-      </c>
-      <c r="Q13" s="80"/>
+      <c r="N13" s="72"/>
+      <c r="O13" s="73"/>
+      <c r="P13" s="72" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q13" s="73"/>
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B14" s="4">
         <v>8</v>
       </c>
-      <c r="C14" s="69"/>
+      <c r="C14" s="62"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G14" s="17">
         <v>7</v>
@@ -2684,20 +2702,20 @@
       <c r="K14" s="16"/>
       <c r="L14" s="16"/>
       <c r="M14" s="16"/>
-      <c r="N14" s="77"/>
-      <c r="O14" s="78"/>
-      <c r="P14" s="57"/>
-      <c r="Q14" s="58"/>
+      <c r="N14" s="70"/>
+      <c r="O14" s="71"/>
+      <c r="P14" s="74"/>
+      <c r="Q14" s="75"/>
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B15" s="4">
         <v>9</v>
       </c>
-      <c r="C15" s="67" t="s">
-        <v>81</v>
+      <c r="C15" s="60" t="s">
+        <v>80</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E15" s="4"/>
       <c r="G15" s="17">
@@ -2709,19 +2727,19 @@
       <c r="K15" s="16"/>
       <c r="L15" s="16"/>
       <c r="M15" s="16"/>
-      <c r="N15" s="55"/>
-      <c r="O15" s="56"/>
-      <c r="P15" s="57"/>
-      <c r="Q15" s="58"/>
+      <c r="N15" s="83"/>
+      <c r="O15" s="84"/>
+      <c r="P15" s="74"/>
+      <c r="Q15" s="75"/>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B16" s="4">
         <v>10</v>
       </c>
-      <c r="C16" s="67"/>
+      <c r="C16" s="60"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G16" s="17"/>
       <c r="H16" s="16"/>
@@ -2730,16 +2748,16 @@
       <c r="K16" s="16"/>
       <c r="L16" s="16"/>
       <c r="M16" s="16"/>
-      <c r="N16" s="55"/>
-      <c r="O16" s="56"/>
-      <c r="P16" s="57"/>
-      <c r="Q16" s="58"/>
+      <c r="N16" s="83"/>
+      <c r="O16" s="84"/>
+      <c r="P16" s="74"/>
+      <c r="Q16" s="75"/>
     </row>
     <row r="17" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B17" s="4">
         <v>11</v>
       </c>
-      <c r="C17" s="67" t="s">
+      <c r="C17" s="60" t="s">
         <v>30</v>
       </c>
       <c r="D17" s="4"/>
@@ -2751,16 +2769,16 @@
       <c r="K17" s="16"/>
       <c r="L17" s="16"/>
       <c r="M17" s="16"/>
-      <c r="N17" s="55"/>
-      <c r="O17" s="56"/>
-      <c r="P17" s="57"/>
-      <c r="Q17" s="58"/>
+      <c r="N17" s="83"/>
+      <c r="O17" s="84"/>
+      <c r="P17" s="74"/>
+      <c r="Q17" s="75"/>
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B18" s="4">
         <v>12</v>
       </c>
-      <c r="C18" s="67"/>
+      <c r="C18" s="60"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="G18" s="17"/>
@@ -2770,16 +2788,16 @@
       <c r="K18" s="16"/>
       <c r="L18" s="16"/>
       <c r="M18" s="16"/>
-      <c r="N18" s="55"/>
-      <c r="O18" s="56"/>
-      <c r="P18" s="57"/>
-      <c r="Q18" s="58"/>
+      <c r="N18" s="83"/>
+      <c r="O18" s="84"/>
+      <c r="P18" s="74"/>
+      <c r="Q18" s="75"/>
     </row>
     <row r="19" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B19" s="4">
         <v>13</v>
       </c>
-      <c r="C19" s="67" t="s">
+      <c r="C19" s="60" t="s">
         <v>30</v>
       </c>
       <c r="D19" s="4"/>
@@ -2791,16 +2809,16 @@
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
-      <c r="N19" s="55"/>
-      <c r="O19" s="56"/>
-      <c r="P19" s="57"/>
-      <c r="Q19" s="58"/>
+      <c r="N19" s="83"/>
+      <c r="O19" s="84"/>
+      <c r="P19" s="74"/>
+      <c r="Q19" s="75"/>
     </row>
     <row r="20" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B20" s="4">
         <v>14</v>
       </c>
-      <c r="C20" s="67"/>
+      <c r="C20" s="60"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
     </row>
@@ -2808,11 +2826,36 @@
       <c r="D22" t="s">
         <v>32</v>
       </c>
-      <c r="F22" s="54"/>
-      <c r="G22" s="54"/>
+      <c r="F22" s="82"/>
+      <c r="G22" s="82"/>
     </row>
   </sheetData>
   <mergeCells count="41">
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="N15:O15"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="P16:Q16"/>
+    <mergeCell ref="P17:Q17"/>
+    <mergeCell ref="N19:O19"/>
+    <mergeCell ref="P18:Q18"/>
+    <mergeCell ref="P19:Q19"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="P15:Q15"/>
+    <mergeCell ref="P8:Q8"/>
+    <mergeCell ref="P9:Q9"/>
+    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="N9:O9"/>
+    <mergeCell ref="I6:O6"/>
+    <mergeCell ref="N8:O8"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="P13:Q13"/>
+    <mergeCell ref="P14:Q14"/>
+    <mergeCell ref="N13:O13"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="N11:O11"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="C19:C20"/>
     <mergeCell ref="C7:C8"/>
@@ -2829,31 +2872,6 @@
     <mergeCell ref="P10:Q10"/>
     <mergeCell ref="P11:Q11"/>
     <mergeCell ref="P12:Q12"/>
-    <mergeCell ref="P13:Q13"/>
-    <mergeCell ref="P14:Q14"/>
-    <mergeCell ref="N13:O13"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="N11:O11"/>
-    <mergeCell ref="P8:Q8"/>
-    <mergeCell ref="P9:Q9"/>
-    <mergeCell ref="N7:O7"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="P6:Q6"/>
-    <mergeCell ref="N9:O9"/>
-    <mergeCell ref="I6:O6"/>
-    <mergeCell ref="N8:O8"/>
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="N15:O15"/>
-    <mergeCell ref="N16:O16"/>
-    <mergeCell ref="N17:O17"/>
-    <mergeCell ref="P16:Q16"/>
-    <mergeCell ref="P17:Q17"/>
-    <mergeCell ref="N19:O19"/>
-    <mergeCell ref="P18:Q18"/>
-    <mergeCell ref="P19:Q19"/>
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="P15:Q15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2866,7 +2884,7 @@
   </sheetPr>
   <dimension ref="B1:R31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
@@ -2891,70 +2909,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="52"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="58"/>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B3" s="133" t="s">
-        <v>72</v>
-      </c>
-      <c r="C3" s="134"/>
-      <c r="D3" s="134"/>
-      <c r="E3" s="134"/>
-      <c r="F3" s="134"/>
-      <c r="G3" s="135"/>
+      <c r="B3" s="52" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" s="53"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="54"/>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.3">
       <c r="E5" s="3"/>
-      <c r="G5" s="74" t="s">
+      <c r="G5" s="67" t="s">
         <v>34</v>
       </c>
-      <c r="H5" s="74"/>
-      <c r="I5" s="74"/>
-      <c r="J5" s="74"/>
-      <c r="K5" s="74"/>
-      <c r="L5" s="74"/>
-      <c r="M5" s="74"/>
-      <c r="N5" s="74"/>
-      <c r="O5" s="74"/>
-      <c r="P5" s="74"/>
-      <c r="Q5" s="74"/>
-      <c r="R5" s="74"/>
+      <c r="H5" s="67"/>
+      <c r="I5" s="67"/>
+      <c r="J5" s="67"/>
+      <c r="K5" s="67"/>
+      <c r="L5" s="67"/>
+      <c r="M5" s="67"/>
+      <c r="N5" s="67"/>
+      <c r="O5" s="67"/>
+      <c r="P5" s="67"/>
+      <c r="Q5" s="67"/>
+      <c r="R5" s="67"/>
     </row>
     <row r="6" spans="2:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="85" t="s">
+      <c r="B6" s="91" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="85"/>
-      <c r="D6" s="85"/>
-      <c r="G6" s="75" t="s">
+      <c r="C6" s="91"/>
+      <c r="D6" s="91"/>
+      <c r="G6" s="68" t="s">
         <v>36</v>
       </c>
-      <c r="H6" s="75" t="s">
+      <c r="H6" s="68" t="s">
         <v>37</v>
       </c>
-      <c r="I6" s="75" t="s">
+      <c r="I6" s="68" t="s">
         <v>38</v>
       </c>
-      <c r="J6" s="61" t="s">
+      <c r="J6" s="78" t="s">
         <v>39</v>
       </c>
-      <c r="K6" s="81" t="s">
+      <c r="K6" s="92" t="s">
         <v>27</v>
       </c>
-      <c r="L6" s="82"/>
-      <c r="M6" s="82"/>
-      <c r="N6" s="82"/>
-      <c r="O6" s="82"/>
-      <c r="P6" s="83"/>
-      <c r="Q6" s="81" t="s">
+      <c r="L6" s="96"/>
+      <c r="M6" s="96"/>
+      <c r="N6" s="96"/>
+      <c r="O6" s="96"/>
+      <c r="P6" s="93"/>
+      <c r="Q6" s="92" t="s">
         <v>28</v>
       </c>
-      <c r="R6" s="83"/>
+      <c r="R6" s="93"/>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B7" s="4" t="s">
@@ -2966,36 +2984,36 @@
       <c r="D7" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G7" s="76"/>
-      <c r="H7" s="76"/>
-      <c r="I7" s="76"/>
-      <c r="J7" s="62"/>
+      <c r="G7" s="69"/>
+      <c r="H7" s="69"/>
+      <c r="I7" s="69"/>
+      <c r="J7" s="79"/>
       <c r="K7" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="L7" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="L7" s="21" t="s">
+      <c r="M7" s="33" t="s">
         <v>85</v>
-      </c>
-      <c r="M7" s="33" t="s">
-        <v>86</v>
       </c>
       <c r="N7" s="33"/>
       <c r="O7" s="21"/>
       <c r="P7" s="21"/>
-      <c r="Q7" s="59" t="s">
+      <c r="Q7" s="76" t="s">
         <v>40</v>
       </c>
-      <c r="R7" s="60"/>
+      <c r="R7" s="77"/>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B8" s="68">
+      <c r="B8" s="61">
         <v>1</v>
       </c>
-      <c r="C8" s="87" t="s">
-        <v>81</v>
+      <c r="C8" s="86" t="s">
+        <v>80</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G8" s="21">
         <v>1</v>
@@ -3004,7 +3022,7 @@
         <v>1</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J8" s="14"/>
       <c r="K8" s="32"/>
@@ -3013,14 +3031,14 @@
       <c r="N8" s="32"/>
       <c r="O8" s="32"/>
       <c r="P8" s="32"/>
-      <c r="Q8" s="79"/>
-      <c r="R8" s="80"/>
+      <c r="Q8" s="72"/>
+      <c r="R8" s="73"/>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B9" s="86"/>
-      <c r="C9" s="88"/>
+      <c r="B9" s="85"/>
+      <c r="C9" s="87"/>
       <c r="D9" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G9" s="17">
         <v>2</v>
@@ -3038,14 +3056,14 @@
       <c r="N9" s="16"/>
       <c r="O9" s="16"/>
       <c r="P9" s="16"/>
-      <c r="Q9" s="65"/>
-      <c r="R9" s="66"/>
+      <c r="Q9" s="94"/>
+      <c r="R9" s="95"/>
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B10" s="86"/>
-      <c r="C10" s="88"/>
+      <c r="B10" s="85"/>
+      <c r="C10" s="87"/>
       <c r="D10" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G10" s="21">
         <v>3</v>
@@ -3063,14 +3081,14 @@
       <c r="N10" s="32"/>
       <c r="O10" s="32"/>
       <c r="P10" s="32"/>
-      <c r="Q10" s="79"/>
-      <c r="R10" s="80"/>
+      <c r="Q10" s="72"/>
+      <c r="R10" s="73"/>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B11" s="86"/>
-      <c r="C11" s="88"/>
+      <c r="B11" s="85"/>
+      <c r="C11" s="87"/>
       <c r="D11" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G11" s="21">
         <v>4</v>
@@ -3088,14 +3106,14 @@
       <c r="N11" s="32"/>
       <c r="O11" s="32"/>
       <c r="P11" s="32"/>
-      <c r="Q11" s="79"/>
-      <c r="R11" s="80"/>
+      <c r="Q11" s="72"/>
+      <c r="R11" s="73"/>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B12" s="86"/>
-      <c r="C12" s="88"/>
+      <c r="B12" s="85"/>
+      <c r="C12" s="87"/>
       <c r="D12" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G12" s="21">
         <v>5</v>
@@ -3113,14 +3131,14 @@
       <c r="N12" s="32"/>
       <c r="O12" s="32"/>
       <c r="P12" s="32"/>
-      <c r="Q12" s="79"/>
-      <c r="R12" s="80"/>
+      <c r="Q12" s="72"/>
+      <c r="R12" s="73"/>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B13" s="69"/>
-      <c r="C13" s="89"/>
+      <c r="B13" s="62"/>
+      <c r="C13" s="88"/>
       <c r="D13" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G13" s="17">
         <v>6</v>
@@ -3130,7 +3148,7 @@
       </c>
       <c r="I13" s="19"/>
       <c r="J13" s="19" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K13" s="20"/>
       <c r="L13" s="16"/>
@@ -3138,18 +3156,18 @@
       <c r="N13" s="16"/>
       <c r="O13" s="16"/>
       <c r="P13" s="16"/>
-      <c r="Q13" s="65"/>
-      <c r="R13" s="66"/>
+      <c r="Q13" s="94"/>
+      <c r="R13" s="95"/>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B14" s="68">
+      <c r="B14" s="61">
         <v>2</v>
       </c>
-      <c r="C14" s="68" t="s">
-        <v>79</v>
+      <c r="C14" s="61" t="s">
+        <v>78</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G14" s="21">
         <v>7</v>
@@ -3167,14 +3185,14 @@
       <c r="N14" s="32"/>
       <c r="O14" s="32"/>
       <c r="P14" s="32"/>
-      <c r="Q14" s="79"/>
-      <c r="R14" s="80"/>
+      <c r="Q14" s="72"/>
+      <c r="R14" s="73"/>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B15" s="86"/>
-      <c r="C15" s="86"/>
+      <c r="B15" s="85"/>
+      <c r="C15" s="85"/>
       <c r="D15" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G15" s="21">
         <v>8</v>
@@ -3192,14 +3210,14 @@
       <c r="N15" s="32"/>
       <c r="O15" s="32"/>
       <c r="P15" s="32"/>
-      <c r="Q15" s="79"/>
-      <c r="R15" s="80"/>
+      <c r="Q15" s="72"/>
+      <c r="R15" s="73"/>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B16" s="86"/>
-      <c r="C16" s="86"/>
+      <c r="B16" s="85"/>
+      <c r="C16" s="85"/>
       <c r="D16" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G16" s="21">
         <v>9</v>
@@ -3217,14 +3235,14 @@
       <c r="N16" s="32"/>
       <c r="O16" s="32"/>
       <c r="P16" s="32"/>
-      <c r="Q16" s="79"/>
-      <c r="R16" s="80"/>
+      <c r="Q16" s="72"/>
+      <c r="R16" s="73"/>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B17" s="86"/>
-      <c r="C17" s="86"/>
+      <c r="B17" s="85"/>
+      <c r="C17" s="85"/>
       <c r="D17" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G17" s="21">
         <v>10</v>
@@ -3242,14 +3260,14 @@
       <c r="N17" s="32"/>
       <c r="O17" s="32"/>
       <c r="P17" s="32"/>
-      <c r="Q17" s="79"/>
-      <c r="R17" s="80"/>
+      <c r="Q17" s="72"/>
+      <c r="R17" s="73"/>
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B18" s="86"/>
-      <c r="C18" s="86"/>
+      <c r="B18" s="85"/>
+      <c r="C18" s="85"/>
       <c r="D18" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G18" s="21">
         <v>11</v>
@@ -3267,14 +3285,14 @@
       <c r="N18" s="32"/>
       <c r="O18" s="32"/>
       <c r="P18" s="32"/>
-      <c r="Q18" s="79"/>
-      <c r="R18" s="80"/>
+      <c r="Q18" s="72"/>
+      <c r="R18" s="73"/>
     </row>
     <row r="19" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B19" s="69"/>
-      <c r="C19" s="69"/>
+      <c r="B19" s="62"/>
+      <c r="C19" s="62"/>
       <c r="D19" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G19" s="21">
         <v>12</v>
@@ -3284,7 +3302,7 @@
       </c>
       <c r="I19" s="14"/>
       <c r="J19" s="19" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K19" s="32"/>
       <c r="L19" s="32"/>
@@ -3292,18 +3310,18 @@
       <c r="N19" s="32"/>
       <c r="O19" s="32"/>
       <c r="P19" s="32"/>
-      <c r="Q19" s="79"/>
-      <c r="R19" s="80"/>
+      <c r="Q19" s="72"/>
+      <c r="R19" s="73"/>
     </row>
     <row r="20" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B20" s="68">
+      <c r="B20" s="61">
         <v>3</v>
       </c>
-      <c r="C20" s="87" t="s">
-        <v>75</v>
+      <c r="C20" s="86" t="s">
+        <v>74</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G20" s="21">
         <v>13</v>
@@ -3321,14 +3339,14 @@
       <c r="N20" s="32"/>
       <c r="O20" s="32"/>
       <c r="P20" s="32"/>
-      <c r="Q20" s="79"/>
-      <c r="R20" s="80"/>
+      <c r="Q20" s="72"/>
+      <c r="R20" s="73"/>
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B21" s="86"/>
-      <c r="C21" s="88"/>
+      <c r="B21" s="85"/>
+      <c r="C21" s="87"/>
       <c r="D21" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G21" s="21">
         <v>14</v>
@@ -3342,7 +3360,7 @@
         <v>1</v>
       </c>
       <c r="L21" s="32" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="M21" s="32">
         <v>10.5</v>
@@ -3350,16 +3368,16 @@
       <c r="N21" s="32"/>
       <c r="O21" s="32"/>
       <c r="P21" s="32"/>
-      <c r="Q21" s="79" t="s">
-        <v>88</v>
-      </c>
-      <c r="R21" s="80"/>
+      <c r="Q21" s="72" t="s">
+        <v>87</v>
+      </c>
+      <c r="R21" s="73"/>
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B22" s="86"/>
-      <c r="C22" s="88"/>
+      <c r="B22" s="85"/>
+      <c r="C22" s="87"/>
       <c r="D22" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G22" s="21">
         <v>15</v>
@@ -3373,7 +3391,7 @@
         <v>1</v>
       </c>
       <c r="L22" s="32" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="M22" s="32">
         <v>10.5</v>
@@ -3381,14 +3399,14 @@
       <c r="N22" s="32"/>
       <c r="O22" s="32"/>
       <c r="P22" s="32"/>
-      <c r="Q22" s="79" t="s">
-        <v>88</v>
-      </c>
-      <c r="R22" s="80"/>
+      <c r="Q22" s="72" t="s">
+        <v>87</v>
+      </c>
+      <c r="R22" s="73"/>
     </row>
     <row r="23" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B23" s="86"/>
-      <c r="C23" s="88"/>
+      <c r="B23" s="85"/>
+      <c r="C23" s="87"/>
       <c r="D23" s="2"/>
       <c r="G23" s="21">
         <v>16</v>
@@ -3402,12 +3420,12 @@
       <c r="N23" s="32"/>
       <c r="O23" s="32"/>
       <c r="P23" s="32"/>
-      <c r="Q23" s="79"/>
-      <c r="R23" s="80"/>
+      <c r="Q23" s="72"/>
+      <c r="R23" s="73"/>
     </row>
     <row r="24" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B24" s="86"/>
-      <c r="C24" s="88"/>
+      <c r="B24" s="85"/>
+      <c r="C24" s="87"/>
       <c r="D24" s="2"/>
       <c r="G24" s="21">
         <v>17</v>
@@ -3421,12 +3439,12 @@
       <c r="N24" s="32"/>
       <c r="O24" s="32"/>
       <c r="P24" s="32"/>
-      <c r="Q24" s="79"/>
-      <c r="R24" s="80"/>
+      <c r="Q24" s="72"/>
+      <c r="R24" s="73"/>
     </row>
     <row r="25" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B25" s="69"/>
-      <c r="C25" s="89"/>
+      <c r="B25" s="62"/>
+      <c r="C25" s="88"/>
       <c r="D25" s="2"/>
       <c r="G25" s="21">
         <v>18</v>
@@ -3440,14 +3458,14 @@
       <c r="N25" s="32"/>
       <c r="O25" s="32"/>
       <c r="P25" s="32"/>
-      <c r="Q25" s="79"/>
-      <c r="R25" s="80"/>
+      <c r="Q25" s="72"/>
+      <c r="R25" s="73"/>
     </row>
     <row r="26" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B26" s="68">
+      <c r="B26" s="61">
         <v>4</v>
       </c>
-      <c r="C26" s="87" t="s">
+      <c r="C26" s="86" t="s">
         <v>30</v>
       </c>
       <c r="D26" s="2" t="s">
@@ -3455,56 +3473,79 @@
       </c>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B27" s="86"/>
-      <c r="C27" s="88"/>
+      <c r="B27" s="85"/>
+      <c r="C27" s="87"/>
       <c r="D27" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="28" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B28" s="86"/>
-      <c r="C28" s="88"/>
+      <c r="B28" s="85"/>
+      <c r="C28" s="87"/>
       <c r="D28" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G28" s="54"/>
-      <c r="H28" s="54"/>
-      <c r="I28" s="84"/>
-      <c r="J28" s="84"/>
-      <c r="K28" s="84"/>
-      <c r="L28" s="84"/>
-      <c r="M28" s="84"/>
+      <c r="G28" s="82"/>
+      <c r="H28" s="82"/>
+      <c r="I28" s="90"/>
+      <c r="J28" s="90"/>
+      <c r="K28" s="90"/>
+      <c r="L28" s="90"/>
+      <c r="M28" s="90"/>
       <c r="N28" s="41"/>
     </row>
     <row r="29" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B29" s="86"/>
-      <c r="C29" s="88"/>
+      <c r="B29" s="85"/>
+      <c r="C29" s="87"/>
       <c r="D29" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="I29" s="90"/>
-      <c r="J29" s="90"/>
-      <c r="K29" s="90"/>
-      <c r="L29" s="90"/>
-      <c r="M29" s="90"/>
+      <c r="I29" s="89"/>
+      <c r="J29" s="89"/>
+      <c r="K29" s="89"/>
+      <c r="L29" s="89"/>
+      <c r="M29" s="89"/>
       <c r="N29" s="42"/>
     </row>
     <row r="30" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B30" s="86"/>
-      <c r="C30" s="88"/>
+      <c r="B30" s="85"/>
+      <c r="C30" s="87"/>
       <c r="D30" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="31" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B31" s="69"/>
-      <c r="C31" s="89"/>
+      <c r="B31" s="62"/>
+      <c r="C31" s="88"/>
       <c r="D31" s="2" t="s">
         <v>30</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="39">
+    <mergeCell ref="Q20:R20"/>
+    <mergeCell ref="Q21:R21"/>
+    <mergeCell ref="Q13:R13"/>
+    <mergeCell ref="K6:P6"/>
+    <mergeCell ref="Q10:R10"/>
+    <mergeCell ref="Q11:R11"/>
+    <mergeCell ref="Q12:R12"/>
+    <mergeCell ref="I28:M28"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="Q6:R6"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="Q25:R25"/>
+    <mergeCell ref="Q14:R14"/>
+    <mergeCell ref="Q15:R15"/>
+    <mergeCell ref="Q22:R22"/>
+    <mergeCell ref="Q23:R23"/>
+    <mergeCell ref="Q24:R24"/>
+    <mergeCell ref="Q16:R16"/>
+    <mergeCell ref="Q17:R17"/>
+    <mergeCell ref="Q18:R18"/>
+    <mergeCell ref="Q8:R8"/>
+    <mergeCell ref="Q9:R9"/>
+    <mergeCell ref="Q19:R19"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="G6:G7"/>
     <mergeCell ref="I6:I7"/>
@@ -3521,29 +3562,6 @@
     <mergeCell ref="G5:R5"/>
     <mergeCell ref="Q7:R7"/>
     <mergeCell ref="G28:H28"/>
-    <mergeCell ref="I28:M28"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="Q6:R6"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="Q25:R25"/>
-    <mergeCell ref="Q14:R14"/>
-    <mergeCell ref="Q15:R15"/>
-    <mergeCell ref="Q22:R22"/>
-    <mergeCell ref="Q23:R23"/>
-    <mergeCell ref="Q24:R24"/>
-    <mergeCell ref="Q16:R16"/>
-    <mergeCell ref="Q17:R17"/>
-    <mergeCell ref="Q18:R18"/>
-    <mergeCell ref="Q8:R8"/>
-    <mergeCell ref="Q9:R9"/>
-    <mergeCell ref="Q19:R19"/>
-    <mergeCell ref="Q20:R20"/>
-    <mergeCell ref="Q21:R21"/>
-    <mergeCell ref="Q13:R13"/>
-    <mergeCell ref="K6:P6"/>
-    <mergeCell ref="Q10:R10"/>
-    <mergeCell ref="Q11:R11"/>
-    <mergeCell ref="Q12:R12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3558,8 +3576,8 @@
   </sheetPr>
   <dimension ref="B1:P21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M28" sqref="M28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3575,75 +3593,75 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="52"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="58"/>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B3" s="127" t="s">
+      <c r="B3" s="112" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="127"/>
-      <c r="D3" s="127"/>
-      <c r="E3" s="127"/>
-      <c r="F3" s="127"/>
-      <c r="G3" s="127"/>
-      <c r="H3" s="127"/>
-      <c r="I3" s="127"/>
-      <c r="J3" s="127"/>
-      <c r="K3" s="127"/>
-      <c r="L3" s="127"/>
-      <c r="M3" s="127"/>
-      <c r="N3" s="127"/>
+      <c r="C3" s="112"/>
+      <c r="D3" s="112"/>
+      <c r="E3" s="112"/>
+      <c r="F3" s="112"/>
+      <c r="G3" s="112"/>
+      <c r="H3" s="112"/>
+      <c r="I3" s="112"/>
+      <c r="J3" s="112"/>
+      <c r="K3" s="112"/>
+      <c r="L3" s="112"/>
+      <c r="M3" s="112"/>
+      <c r="N3" s="112"/>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B4" s="75" t="s">
+      <c r="B4" s="68" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="121" t="s">
+      <c r="C4" s="104" t="s">
         <v>43</v>
       </c>
-      <c r="D4" s="103" t="s">
+      <c r="D4" s="117" t="s">
         <v>44</v>
       </c>
-      <c r="E4" s="61" t="s">
+      <c r="E4" s="78" t="s">
         <v>45</v>
       </c>
-      <c r="F4" s="59" t="s">
+      <c r="F4" s="76" t="s">
         <v>27</v>
       </c>
-      <c r="G4" s="64"/>
-      <c r="H4" s="64"/>
-      <c r="I4" s="64"/>
-      <c r="J4" s="64"/>
-      <c r="K4" s="64"/>
-      <c r="L4" s="60"/>
-      <c r="M4" s="63" t="s">
+      <c r="G4" s="81"/>
+      <c r="H4" s="81"/>
+      <c r="I4" s="81"/>
+      <c r="J4" s="81"/>
+      <c r="K4" s="81"/>
+      <c r="L4" s="77"/>
+      <c r="M4" s="80" t="s">
         <v>28</v>
       </c>
-      <c r="N4" s="63"/>
+      <c r="N4" s="80"/>
     </row>
     <row r="5" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="102"/>
-      <c r="C5" s="122"/>
-      <c r="D5" s="104"/>
-      <c r="E5" s="120"/>
+      <c r="B5" s="116"/>
+      <c r="C5" s="105"/>
+      <c r="D5" s="118"/>
+      <c r="E5" s="103"/>
       <c r="F5" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="G5" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="G5" s="21" t="s">
+      <c r="H5" s="21" t="s">
         <v>85</v>
-      </c>
-      <c r="H5" s="21" t="s">
-        <v>86</v>
       </c>
       <c r="I5" s="24"/>
       <c r="J5" s="24"/>
-      <c r="K5" s="116"/>
-      <c r="L5" s="117"/>
+      <c r="K5" s="99"/>
+      <c r="L5" s="100"/>
       <c r="M5" s="24" t="s">
         <v>29</v>
       </c>
@@ -3651,11 +3669,11 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="2:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:14" ht="43.8" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B6" s="22">
         <v>1</v>
       </c>
-      <c r="C6" s="100" t="s">
+      <c r="C6" s="114" t="s">
         <v>47</v>
       </c>
       <c r="D6" s="28" t="s">
@@ -3665,31 +3683,31 @@
         <v>31</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G6" s="32" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H6" s="32" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I6" s="27"/>
       <c r="J6" s="27"/>
-      <c r="K6" s="131"/>
-      <c r="L6" s="132"/>
+      <c r="K6" s="101"/>
+      <c r="L6" s="102"/>
       <c r="M6" s="27" t="s">
-        <v>88</v>
-      </c>
-      <c r="N6" s="22" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
+        <v>87</v>
+      </c>
+      <c r="N6" s="136" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B7" s="10">
         <f>B6+1</f>
         <v>2</v>
       </c>
-      <c r="C7" s="100"/>
+      <c r="C7" s="114"/>
       <c r="D7" s="29" t="s">
         <v>49</v>
       </c>
@@ -3697,31 +3715,31 @@
         <v>31</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G7" s="32" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H7" s="32" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
-      <c r="K7" s="123"/>
-      <c r="L7" s="124"/>
+      <c r="K7" s="106"/>
+      <c r="L7" s="107"/>
       <c r="M7" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="N7" s="10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+      <c r="N7" s="137" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B8" s="10">
         <f t="shared" ref="B8:B13" si="0">B7+1</f>
         <v>3</v>
       </c>
-      <c r="C8" s="100"/>
+      <c r="C8" s="114"/>
       <c r="D8" s="29" t="s">
         <v>50</v>
       </c>
@@ -3729,74 +3747,74 @@
         <v>31</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G8" s="32" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H8" s="32" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
       <c r="K8" s="6"/>
       <c r="L8" s="6"/>
       <c r="M8" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="N8" s="10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+      <c r="N8" s="137" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" ht="72" x14ac:dyDescent="0.3">
       <c r="B9" s="10">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C9" s="100"/>
+      <c r="C9" s="114"/>
       <c r="D9" s="29" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E9" s="10" t="s">
         <v>31</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G9" s="32" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H9" s="32" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I9" s="10"/>
       <c r="J9" s="10"/>
-      <c r="K9" s="125"/>
-      <c r="L9" s="126"/>
+      <c r="K9" s="108"/>
+      <c r="L9" s="109"/>
       <c r="M9" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="N9" s="10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+      <c r="N9" s="137" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B10" s="10">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C10" s="100"/>
+      <c r="C10" s="114"/>
       <c r="D10" s="29" t="s">
         <v>31</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F10" s="32">
         <v>1</v>
       </c>
       <c r="G10" s="32" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H10" s="32">
         <v>10.5</v>
@@ -3804,31 +3822,31 @@
       <c r="I10" s="32"/>
       <c r="J10" s="32"/>
       <c r="K10" s="32"/>
-      <c r="L10" s="79" t="s">
-        <v>88</v>
-      </c>
-      <c r="M10" s="80"/>
-      <c r="N10" s="10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="L10" s="72" t="s">
+        <v>87</v>
+      </c>
+      <c r="M10" s="73"/>
+      <c r="N10" s="137" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B11" s="10">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C11" s="100"/>
+      <c r="C11" s="114"/>
       <c r="D11" s="29" t="s">
         <v>31</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F11" s="32">
         <v>1</v>
       </c>
       <c r="G11" s="32" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H11" s="32">
         <v>10.5</v>
@@ -3836,12 +3854,12 @@
       <c r="I11" s="32"/>
       <c r="J11" s="32"/>
       <c r="K11" s="32"/>
-      <c r="L11" s="79" t="s">
-        <v>88</v>
-      </c>
-      <c r="M11" s="80"/>
-      <c r="N11" s="10" t="s">
-        <v>30</v>
+      <c r="L11" s="72" t="s">
+        <v>87</v>
+      </c>
+      <c r="M11" s="73"/>
+      <c r="N11" s="137" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.3">
@@ -3849,7 +3867,7 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C12" s="100"/>
+      <c r="C12" s="114"/>
       <c r="D12" s="29"/>
       <c r="E12" s="10"/>
       <c r="F12" s="13"/>
@@ -3857,17 +3875,17 @@
       <c r="H12" s="9"/>
       <c r="I12" s="9"/>
       <c r="J12" s="9"/>
-      <c r="K12" s="118"/>
-      <c r="L12" s="119"/>
+      <c r="K12" s="110"/>
+      <c r="L12" s="111"/>
       <c r="M12" s="5"/>
-      <c r="N12" s="10"/>
+      <c r="N12" s="137"/>
     </row>
     <row r="13" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="23">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C13" s="101"/>
+      <c r="C13" s="115"/>
       <c r="D13" s="30"/>
       <c r="E13" s="23"/>
       <c r="F13" s="23"/>
@@ -3875,10 +3893,10 @@
       <c r="H13" s="23"/>
       <c r="I13" s="23"/>
       <c r="J13" s="23"/>
-      <c r="K13" s="114"/>
-      <c r="L13" s="115"/>
+      <c r="K13" s="97"/>
+      <c r="L13" s="98"/>
       <c r="M13" s="23"/>
-      <c r="N13" s="23"/>
+      <c r="N13" s="138"/>
     </row>
     <row r="14" spans="2:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B14" s="25"/>
@@ -3907,98 +3925,98 @@
       <c r="H15" s="7"/>
       <c r="I15" s="7"/>
       <c r="J15" s="7"/>
-      <c r="K15" s="99"/>
-      <c r="L15" s="99"/>
+      <c r="K15" s="113"/>
+      <c r="L15" s="113"/>
       <c r="M15" s="7"/>
     </row>
     <row r="16" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="M16" s="7"/>
     </row>
     <row r="17" spans="2:16" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="C17" s="93" t="s">
+      <c r="C17" s="125" t="s">
         <v>52</v>
       </c>
-      <c r="D17" s="95"/>
-      <c r="E17" s="95"/>
-      <c r="F17" s="96"/>
+      <c r="D17" s="126"/>
+      <c r="E17" s="126"/>
+      <c r="F17" s="127"/>
       <c r="G17" s="37" t="s">
         <v>53</v>
       </c>
-      <c r="H17" s="93" t="s">
+      <c r="H17" s="125" t="s">
         <v>54</v>
       </c>
-      <c r="I17" s="94"/>
-      <c r="J17" s="95"/>
-      <c r="K17" s="95"/>
-      <c r="L17" s="96"/>
-      <c r="M17" s="93" t="s">
+      <c r="I17" s="128"/>
+      <c r="J17" s="126"/>
+      <c r="K17" s="126"/>
+      <c r="L17" s="127"/>
+      <c r="M17" s="125" t="s">
         <v>55</v>
       </c>
-      <c r="N17" s="94"/>
-      <c r="O17" s="95"/>
-      <c r="P17" s="96"/>
+      <c r="N17" s="128"/>
+      <c r="O17" s="126"/>
+      <c r="P17" s="127"/>
     </row>
     <row r="18" spans="2:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="107" t="s">
+      <c r="B18" s="121" t="s">
         <v>43</v>
       </c>
-      <c r="C18" s="108" t="s">
+      <c r="C18" s="122" t="s">
         <v>56</v>
       </c>
-      <c r="D18" s="92" t="s">
+      <c r="D18" s="123" t="s">
         <v>57</v>
       </c>
-      <c r="E18" s="92" t="s">
+      <c r="E18" s="123" t="s">
         <v>58</v>
       </c>
-      <c r="F18" s="91" t="s">
+      <c r="F18" s="124" t="s">
         <v>59</v>
       </c>
-      <c r="G18" s="113" t="s">
+      <c r="G18" s="133" t="s">
         <v>60</v>
       </c>
-      <c r="H18" s="109" t="s">
+      <c r="H18" s="129" t="s">
         <v>61</v>
       </c>
-      <c r="I18" s="110"/>
-      <c r="J18" s="92" t="s">
+      <c r="I18" s="130"/>
+      <c r="J18" s="123" t="s">
         <v>56</v>
       </c>
-      <c r="K18" s="92" t="s">
+      <c r="K18" s="123" t="s">
         <v>57</v>
       </c>
-      <c r="L18" s="91" t="s">
+      <c r="L18" s="124" t="s">
         <v>58</v>
       </c>
-      <c r="M18" s="97" t="s">
+      <c r="M18" s="134" t="s">
         <v>61</v>
       </c>
-      <c r="N18" s="92" t="s">
+      <c r="N18" s="123" t="s">
         <v>56</v>
       </c>
-      <c r="O18" s="92" t="s">
+      <c r="O18" s="123" t="s">
         <v>57</v>
       </c>
-      <c r="P18" s="91" t="s">
+      <c r="P18" s="124" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B19" s="107"/>
-      <c r="C19" s="108"/>
-      <c r="D19" s="92"/>
-      <c r="E19" s="92"/>
-      <c r="F19" s="91"/>
-      <c r="G19" s="113"/>
-      <c r="H19" s="111"/>
-      <c r="I19" s="112"/>
-      <c r="J19" s="92"/>
-      <c r="K19" s="92"/>
-      <c r="L19" s="91"/>
-      <c r="M19" s="98"/>
-      <c r="N19" s="92"/>
-      <c r="O19" s="92"/>
-      <c r="P19" s="91"/>
+      <c r="B19" s="121"/>
+      <c r="C19" s="122"/>
+      <c r="D19" s="123"/>
+      <c r="E19" s="123"/>
+      <c r="F19" s="124"/>
+      <c r="G19" s="133"/>
+      <c r="H19" s="131"/>
+      <c r="I19" s="132"/>
+      <c r="J19" s="123"/>
+      <c r="K19" s="123"/>
+      <c r="L19" s="124"/>
+      <c r="M19" s="135"/>
+      <c r="N19" s="123"/>
+      <c r="O19" s="123"/>
+      <c r="P19" s="124"/>
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B20" s="40" t="s">
@@ -4008,34 +4026,36 @@
         <v>8</v>
       </c>
       <c r="D20" s="38">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E20" s="38">
-        <v>3</v>
-      </c>
-      <c r="F20" s="39"/>
+        <v>0</v>
+      </c>
+      <c r="F20" s="39">
+        <v>0</v>
+      </c>
       <c r="G20" s="44"/>
-      <c r="H20" s="105" t="s">
-        <v>62</v>
-      </c>
-      <c r="I20" s="106"/>
+      <c r="H20" s="119" t="s">
+        <v>119</v>
+      </c>
+      <c r="I20" s="120"/>
       <c r="J20" s="2">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K20" s="38">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L20" s="39">
         <v>0</v>
       </c>
       <c r="M20" s="43" t="s">
-        <v>62</v>
+        <v>119</v>
       </c>
       <c r="N20" s="2">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="O20" s="38">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="P20" s="39">
         <v>0</v>
@@ -4046,20 +4066,12 @@
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="L11:M11"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="F4:L4"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="B3:N3"/>
-    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="L18:L19"/>
+    <mergeCell ref="O18:O19"/>
+    <mergeCell ref="P18:P19"/>
+    <mergeCell ref="M17:P17"/>
+    <mergeCell ref="M18:M19"/>
+    <mergeCell ref="N18:N19"/>
     <mergeCell ref="K15:L15"/>
     <mergeCell ref="C6:C13"/>
     <mergeCell ref="B4:B5"/>
@@ -4076,12 +4088,20 @@
     <mergeCell ref="H18:I19"/>
     <mergeCell ref="G18:G19"/>
     <mergeCell ref="K18:K19"/>
-    <mergeCell ref="L18:L19"/>
-    <mergeCell ref="O18:O19"/>
-    <mergeCell ref="P18:P19"/>
-    <mergeCell ref="M17:P17"/>
-    <mergeCell ref="M18:M19"/>
-    <mergeCell ref="N18:N19"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="F4:L4"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="B3:N3"/>
+    <mergeCell ref="L10:M10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4090,21 +4110,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010058284A30843C9F43BD758DDD8294D484" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6d50638930d08c51b5585735b2be047e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="fed1744a-f275-4023-9290-77fd546fd730" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4acb07121b76573bb3c966f3dcb1b903" ns2:_="">
     <xsd:import namespace="fed1744a-f275-4023-9290-77fd546fd730"/>
@@ -4248,24 +4253,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF0EB622-FDCF-4321-9FF5-C0B282D1670E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2BC1EB47-4FFF-47F3-894F-DED91590EA19}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33EFF49E-866D-4BFD-B7FD-9BB436667B53}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4281,4 +4284,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2BC1EB47-4FFF-47F3-894F-DED91590EA19}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF0EB622-FDCF-4321-9FF5-C0B282D1670E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added TestLink automatically generated docs
</commit_message>
<xml_diff>
--- a/Docs/Lab02/Lab02_BBT_TCs_Form.xlsx
+++ b/Docs/Lab02/Lab02_BBT_TCs_Form.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28526"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF56910B-2C44-4430-9E9E-203F7F9089BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F77E6DD8-CB3F-4BA1-A820-4C82863556DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1625,6 +1625,45 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1661,43 +1700,25 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1715,26 +1736,74 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1783,75 +1852,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2409,7 +2409,7 @@
   </sheetPr>
   <dimension ref="B1:Q22"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
@@ -2440,35 +2440,35 @@
       <c r="E1" s="60"/>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B3" s="65" t="s">
+      <c r="B3" s="78" t="s">
         <v>71</v>
       </c>
-      <c r="C3" s="66"/>
-      <c r="D3" s="66"/>
-      <c r="E3" s="66"/>
-      <c r="F3" s="66"/>
-      <c r="G3" s="67"/>
+      <c r="C3" s="79"/>
+      <c r="D3" s="79"/>
+      <c r="E3" s="79"/>
+      <c r="F3" s="79"/>
+      <c r="G3" s="80"/>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B5" s="68" t="s">
+      <c r="B5" s="81" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="68"/>
-      <c r="D5" s="68"/>
-      <c r="E5" s="68"/>
-      <c r="G5" s="69" t="s">
+      <c r="C5" s="81"/>
+      <c r="D5" s="81"/>
+      <c r="E5" s="81"/>
+      <c r="G5" s="82" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="69"/>
-      <c r="I5" s="69"/>
-      <c r="J5" s="69"/>
-      <c r="K5" s="69"/>
-      <c r="L5" s="69"/>
-      <c r="M5" s="69"/>
-      <c r="N5" s="69"/>
-      <c r="O5" s="69"/>
-      <c r="P5" s="69"/>
-      <c r="Q5" s="69"/>
+      <c r="H5" s="82"/>
+      <c r="I5" s="82"/>
+      <c r="J5" s="82"/>
+      <c r="K5" s="82"/>
+      <c r="L5" s="82"/>
+      <c r="M5" s="82"/>
+      <c r="N5" s="82"/>
+      <c r="O5" s="82"/>
+      <c r="P5" s="82"/>
+      <c r="Q5" s="82"/>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B6" s="21" t="s">
@@ -2483,39 +2483,39 @@
       <c r="E6" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="70" t="s">
+      <c r="G6" s="83" t="s">
         <v>25</v>
       </c>
-      <c r="H6" s="80" t="s">
+      <c r="H6" s="71" t="s">
         <v>26</v>
       </c>
-      <c r="I6" s="78" t="s">
+      <c r="I6" s="69" t="s">
         <v>27</v>
       </c>
-      <c r="J6" s="83"/>
-      <c r="K6" s="83"/>
-      <c r="L6" s="83"/>
-      <c r="M6" s="83"/>
-      <c r="N6" s="83"/>
-      <c r="O6" s="79"/>
-      <c r="P6" s="82" t="s">
+      <c r="J6" s="74"/>
+      <c r="K6" s="74"/>
+      <c r="L6" s="74"/>
+      <c r="M6" s="74"/>
+      <c r="N6" s="74"/>
+      <c r="O6" s="70"/>
+      <c r="P6" s="73" t="s">
         <v>28</v>
       </c>
-      <c r="Q6" s="82"/>
+      <c r="Q6" s="73"/>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B7" s="4">
         <v>1</v>
       </c>
-      <c r="C7" s="62" t="s">
+      <c r="C7" s="75" t="s">
         <v>72</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>72</v>
       </c>
       <c r="E7" s="4"/>
-      <c r="G7" s="71"/>
-      <c r="H7" s="81"/>
+      <c r="G7" s="84"/>
+      <c r="H7" s="72"/>
       <c r="I7" s="21" t="s">
         <v>83</v>
       </c>
@@ -2527,18 +2527,18 @@
       </c>
       <c r="L7" s="21"/>
       <c r="M7" s="21"/>
-      <c r="N7" s="78"/>
-      <c r="O7" s="79"/>
-      <c r="P7" s="78" t="s">
+      <c r="N7" s="69"/>
+      <c r="O7" s="70"/>
+      <c r="P7" s="69" t="s">
         <v>29</v>
       </c>
-      <c r="Q7" s="79"/>
+      <c r="Q7" s="70"/>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B8" s="4">
         <v>2</v>
       </c>
-      <c r="C8" s="62"/>
+      <c r="C8" s="75"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4" t="s">
         <v>73</v>
@@ -2560,18 +2560,18 @@
       </c>
       <c r="L8" s="32"/>
       <c r="M8" s="32"/>
-      <c r="N8" s="74"/>
-      <c r="O8" s="75"/>
-      <c r="P8" s="74" t="s">
+      <c r="N8" s="67"/>
+      <c r="O8" s="68"/>
+      <c r="P8" s="67" t="s">
         <v>87</v>
       </c>
-      <c r="Q8" s="75"/>
+      <c r="Q8" s="68"/>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B9" s="4">
         <v>3</v>
       </c>
-      <c r="C9" s="62" t="s">
+      <c r="C9" s="75" t="s">
         <v>74</v>
       </c>
       <c r="D9" s="4" t="s">
@@ -2589,18 +2589,18 @@
       <c r="K9" s="32"/>
       <c r="L9" s="32"/>
       <c r="M9" s="32"/>
-      <c r="N9" s="74"/>
-      <c r="O9" s="75"/>
-      <c r="P9" s="74" t="s">
+      <c r="N9" s="67"/>
+      <c r="O9" s="68"/>
+      <c r="P9" s="67" t="s">
         <v>90</v>
       </c>
-      <c r="Q9" s="75"/>
+      <c r="Q9" s="68"/>
     </row>
     <row r="10" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B10" s="4">
         <v>4</v>
       </c>
-      <c r="C10" s="62"/>
+      <c r="C10" s="75"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4" t="s">
         <v>75</v>
@@ -2622,18 +2622,18 @@
       </c>
       <c r="L10" s="32"/>
       <c r="M10" s="32"/>
-      <c r="N10" s="74"/>
-      <c r="O10" s="75"/>
-      <c r="P10" s="74" t="s">
+      <c r="N10" s="67"/>
+      <c r="O10" s="68"/>
+      <c r="P10" s="67" t="s">
         <v>88</v>
       </c>
-      <c r="Q10" s="75"/>
+      <c r="Q10" s="68"/>
     </row>
     <row r="11" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="4">
         <v>5</v>
       </c>
-      <c r="C11" s="62" t="s">
+      <c r="C11" s="75" t="s">
         <v>76</v>
       </c>
       <c r="D11" s="4" t="s">
@@ -2651,18 +2651,18 @@
       <c r="K11" s="32"/>
       <c r="L11" s="32"/>
       <c r="M11" s="32"/>
-      <c r="N11" s="74"/>
-      <c r="O11" s="75"/>
-      <c r="P11" s="74" t="s">
+      <c r="N11" s="67"/>
+      <c r="O11" s="68"/>
+      <c r="P11" s="67" t="s">
         <v>90</v>
       </c>
-      <c r="Q11" s="75"/>
+      <c r="Q11" s="68"/>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B12" s="4">
         <v>6</v>
       </c>
-      <c r="C12" s="62"/>
+      <c r="C12" s="75"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4" t="s">
         <v>77</v>
@@ -2686,16 +2686,16 @@
       <c r="M12" s="32"/>
       <c r="N12" s="32"/>
       <c r="O12" s="32"/>
-      <c r="P12" s="74" t="s">
+      <c r="P12" s="67" t="s">
         <v>88</v>
       </c>
-      <c r="Q12" s="75"/>
+      <c r="Q12" s="68"/>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B13" s="4">
         <v>7</v>
       </c>
-      <c r="C13" s="63" t="s">
+      <c r="C13" s="76" t="s">
         <v>78</v>
       </c>
       <c r="D13" s="4" t="s">
@@ -2719,18 +2719,18 @@
       </c>
       <c r="L13" s="32"/>
       <c r="M13" s="32"/>
-      <c r="N13" s="74"/>
-      <c r="O13" s="75"/>
-      <c r="P13" s="74" t="s">
+      <c r="N13" s="67"/>
+      <c r="O13" s="68"/>
+      <c r="P13" s="67" t="s">
         <v>88</v>
       </c>
-      <c r="Q13" s="75"/>
+      <c r="Q13" s="68"/>
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B14" s="4">
         <v>8</v>
       </c>
-      <c r="C14" s="64"/>
+      <c r="C14" s="77"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4" t="s">
         <v>79</v>
@@ -2752,18 +2752,18 @@
       </c>
       <c r="L14" s="16"/>
       <c r="M14" s="16"/>
-      <c r="N14" s="72"/>
-      <c r="O14" s="73"/>
-      <c r="P14" s="76" t="s">
+      <c r="N14" s="85"/>
+      <c r="O14" s="86"/>
+      <c r="P14" s="65" t="s">
         <v>88</v>
       </c>
-      <c r="Q14" s="77"/>
+      <c r="Q14" s="66"/>
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B15" s="4">
         <v>9</v>
       </c>
-      <c r="C15" s="62" t="s">
+      <c r="C15" s="75" t="s">
         <v>80</v>
       </c>
       <c r="D15" s="4" t="s">
@@ -2779,16 +2779,16 @@
       <c r="K15" s="16"/>
       <c r="L15" s="16"/>
       <c r="M15" s="16"/>
-      <c r="N15" s="85"/>
-      <c r="O15" s="86"/>
-      <c r="P15" s="76"/>
-      <c r="Q15" s="77"/>
+      <c r="N15" s="63"/>
+      <c r="O15" s="64"/>
+      <c r="P15" s="65"/>
+      <c r="Q15" s="66"/>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B16" s="4">
         <v>10</v>
       </c>
-      <c r="C16" s="62"/>
+      <c r="C16" s="75"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4" t="s">
         <v>81</v>
@@ -2800,16 +2800,16 @@
       <c r="K16" s="16"/>
       <c r="L16" s="16"/>
       <c r="M16" s="16"/>
-      <c r="N16" s="85"/>
-      <c r="O16" s="86"/>
-      <c r="P16" s="76"/>
-      <c r="Q16" s="77"/>
+      <c r="N16" s="63"/>
+      <c r="O16" s="64"/>
+      <c r="P16" s="65"/>
+      <c r="Q16" s="66"/>
     </row>
     <row r="17" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B17" s="4">
         <v>11</v>
       </c>
-      <c r="C17" s="62" t="s">
+      <c r="C17" s="75" t="s">
         <v>119</v>
       </c>
       <c r="D17" s="4" t="s">
@@ -2823,16 +2823,16 @@
       <c r="K17" s="16"/>
       <c r="L17" s="16"/>
       <c r="M17" s="16"/>
-      <c r="N17" s="85"/>
-      <c r="O17" s="86"/>
-      <c r="P17" s="76"/>
-      <c r="Q17" s="77"/>
+      <c r="N17" s="63"/>
+      <c r="O17" s="64"/>
+      <c r="P17" s="65"/>
+      <c r="Q17" s="66"/>
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B18" s="4">
         <v>12</v>
       </c>
-      <c r="C18" s="62"/>
+      <c r="C18" s="75"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4" t="s">
         <v>120</v>
@@ -2844,16 +2844,16 @@
       <c r="K18" s="16"/>
       <c r="L18" s="16"/>
       <c r="M18" s="16"/>
-      <c r="N18" s="85"/>
-      <c r="O18" s="86"/>
-      <c r="P18" s="76"/>
-      <c r="Q18" s="77"/>
+      <c r="N18" s="63"/>
+      <c r="O18" s="64"/>
+      <c r="P18" s="65"/>
+      <c r="Q18" s="66"/>
     </row>
     <row r="19" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B19" s="4">
         <v>13</v>
       </c>
-      <c r="C19" s="62" t="s">
+      <c r="C19" s="75" t="s">
         <v>30</v>
       </c>
       <c r="D19" s="4"/>
@@ -2865,16 +2865,16 @@
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
-      <c r="N19" s="85"/>
-      <c r="O19" s="86"/>
-      <c r="P19" s="76"/>
-      <c r="Q19" s="77"/>
+      <c r="N19" s="63"/>
+      <c r="O19" s="64"/>
+      <c r="P19" s="65"/>
+      <c r="Q19" s="66"/>
     </row>
     <row r="20" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B20" s="4">
         <v>14</v>
       </c>
-      <c r="C20" s="62"/>
+      <c r="C20" s="75"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
     </row>
@@ -2882,36 +2882,11 @@
       <c r="D22" t="s">
         <v>32</v>
       </c>
-      <c r="F22" s="84"/>
-      <c r="G22" s="84"/>
+      <c r="F22" s="62"/>
+      <c r="G22" s="62"/>
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="N15:O15"/>
-    <mergeCell ref="N16:O16"/>
-    <mergeCell ref="N17:O17"/>
-    <mergeCell ref="P16:Q16"/>
-    <mergeCell ref="P17:Q17"/>
-    <mergeCell ref="N19:O19"/>
-    <mergeCell ref="P18:Q18"/>
-    <mergeCell ref="P19:Q19"/>
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="P15:Q15"/>
-    <mergeCell ref="P8:Q8"/>
-    <mergeCell ref="P9:Q9"/>
-    <mergeCell ref="N7:O7"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="P6:Q6"/>
-    <mergeCell ref="N9:O9"/>
-    <mergeCell ref="I6:O6"/>
-    <mergeCell ref="N8:O8"/>
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="P13:Q13"/>
-    <mergeCell ref="P14:Q14"/>
-    <mergeCell ref="N13:O13"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="N11:O11"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="C19:C20"/>
     <mergeCell ref="C7:C8"/>
@@ -2928,6 +2903,31 @@
     <mergeCell ref="P10:Q10"/>
     <mergeCell ref="P11:Q11"/>
     <mergeCell ref="P12:Q12"/>
+    <mergeCell ref="P13:Q13"/>
+    <mergeCell ref="P14:Q14"/>
+    <mergeCell ref="N13:O13"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="P8:Q8"/>
+    <mergeCell ref="P9:Q9"/>
+    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="N9:O9"/>
+    <mergeCell ref="I6:O6"/>
+    <mergeCell ref="N8:O8"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="N15:O15"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="P16:Q16"/>
+    <mergeCell ref="P17:Q17"/>
+    <mergeCell ref="N19:O19"/>
+    <mergeCell ref="P18:Q18"/>
+    <mergeCell ref="P19:Q19"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="P15:Q15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2940,7 +2940,7 @@
   </sheetPr>
   <dimension ref="B1:R31"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="92" workbookViewId="0">
+    <sheetView topLeftCell="D4" zoomScale="92" workbookViewId="0">
       <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
@@ -2983,47 +2983,47 @@
       <c r="G3" s="54"/>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="G4" s="69" t="s">
+      <c r="G4" s="82" t="s">
         <v>34</v>
       </c>
-      <c r="H4" s="69"/>
-      <c r="I4" s="69"/>
-      <c r="J4" s="69"/>
-      <c r="K4" s="69"/>
-      <c r="L4" s="69"/>
-      <c r="M4" s="69"/>
-      <c r="N4" s="69"/>
-      <c r="O4" s="69"/>
-      <c r="P4" s="69"/>
-      <c r="Q4" s="69"/>
-      <c r="R4" s="69"/>
+      <c r="H4" s="82"/>
+      <c r="I4" s="82"/>
+      <c r="J4" s="82"/>
+      <c r="K4" s="82"/>
+      <c r="L4" s="82"/>
+      <c r="M4" s="82"/>
+      <c r="N4" s="82"/>
+      <c r="O4" s="82"/>
+      <c r="P4" s="82"/>
+      <c r="Q4" s="82"/>
+      <c r="R4" s="82"/>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.3">
       <c r="E5" s="3"/>
-      <c r="G5" s="70" t="s">
+      <c r="G5" s="83" t="s">
         <v>36</v>
       </c>
-      <c r="H5" s="70" t="s">
+      <c r="H5" s="83" t="s">
         <v>37</v>
       </c>
-      <c r="I5" s="70" t="s">
+      <c r="I5" s="83" t="s">
         <v>38</v>
       </c>
-      <c r="J5" s="80" t="s">
+      <c r="J5" s="71" t="s">
         <v>39</v>
       </c>
-      <c r="K5" s="94" t="s">
+      <c r="K5" s="89" t="s">
         <v>27</v>
       </c>
-      <c r="L5" s="98"/>
-      <c r="M5" s="98"/>
-      <c r="N5" s="98"/>
-      <c r="O5" s="98"/>
-      <c r="P5" s="95"/>
-      <c r="Q5" s="94" t="s">
+      <c r="L5" s="90"/>
+      <c r="M5" s="90"/>
+      <c r="N5" s="90"/>
+      <c r="O5" s="90"/>
+      <c r="P5" s="91"/>
+      <c r="Q5" s="89" t="s">
         <v>28</v>
       </c>
-      <c r="R5" s="95"/>
+      <c r="R5" s="91"/>
     </row>
     <row r="6" spans="2:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="93" t="s">
@@ -3031,10 +3031,10 @@
       </c>
       <c r="C6" s="93"/>
       <c r="D6" s="93"/>
-      <c r="G6" s="71"/>
-      <c r="H6" s="71"/>
-      <c r="I6" s="71"/>
-      <c r="J6" s="81"/>
+      <c r="G6" s="84"/>
+      <c r="H6" s="84"/>
+      <c r="I6" s="84"/>
+      <c r="J6" s="72"/>
       <c r="K6" s="21" t="s">
         <v>83</v>
       </c>
@@ -3047,10 +3047,10 @@
       <c r="N6" s="33"/>
       <c r="O6" s="21"/>
       <c r="P6" s="21"/>
-      <c r="Q6" s="78" t="s">
+      <c r="Q6" s="69" t="s">
         <v>40</v>
       </c>
-      <c r="R6" s="79"/>
+      <c r="R6" s="70"/>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B7" s="4" t="s">
@@ -3078,14 +3078,14 @@
       <c r="N7" s="32"/>
       <c r="O7" s="32"/>
       <c r="P7" s="32"/>
-      <c r="Q7" s="74"/>
-      <c r="R7" s="75"/>
+      <c r="Q7" s="67"/>
+      <c r="R7" s="68"/>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B8" s="63">
+      <c r="B8" s="76">
         <v>1</v>
       </c>
-      <c r="C8" s="88" t="s">
+      <c r="C8" s="95" t="s">
         <v>127</v>
       </c>
       <c r="D8" s="2" t="s">
@@ -3107,12 +3107,12 @@
       <c r="N8" s="16"/>
       <c r="O8" s="16"/>
       <c r="P8" s="16"/>
-      <c r="Q8" s="96"/>
-      <c r="R8" s="97"/>
+      <c r="Q8" s="87"/>
+      <c r="R8" s="88"/>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B9" s="87"/>
-      <c r="C9" s="89"/>
+      <c r="B9" s="94"/>
+      <c r="C9" s="96"/>
       <c r="D9" s="2" t="s">
         <v>95</v>
       </c>
@@ -3132,12 +3132,12 @@
       <c r="N9" s="32"/>
       <c r="O9" s="32"/>
       <c r="P9" s="32"/>
-      <c r="Q9" s="74"/>
-      <c r="R9" s="75"/>
+      <c r="Q9" s="67"/>
+      <c r="R9" s="68"/>
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B10" s="87"/>
-      <c r="C10" s="89"/>
+      <c r="B10" s="94"/>
+      <c r="C10" s="96"/>
       <c r="D10" s="2" t="s">
         <v>98</v>
       </c>
@@ -3157,12 +3157,12 @@
       <c r="N10" s="32"/>
       <c r="O10" s="32"/>
       <c r="P10" s="32"/>
-      <c r="Q10" s="74"/>
-      <c r="R10" s="75"/>
+      <c r="Q10" s="67"/>
+      <c r="R10" s="68"/>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B11" s="87"/>
-      <c r="C11" s="89"/>
+      <c r="B11" s="94"/>
+      <c r="C11" s="96"/>
       <c r="D11" s="2" t="s">
         <v>131</v>
       </c>
@@ -3182,12 +3182,12 @@
       <c r="N11" s="32"/>
       <c r="O11" s="32"/>
       <c r="P11" s="32"/>
-      <c r="Q11" s="74"/>
-      <c r="R11" s="75"/>
+      <c r="Q11" s="67"/>
+      <c r="R11" s="68"/>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B12" s="87"/>
-      <c r="C12" s="89"/>
+      <c r="B12" s="94"/>
+      <c r="C12" s="96"/>
       <c r="D12" s="2" t="s">
         <v>132</v>
       </c>
@@ -3207,12 +3207,12 @@
       <c r="N12" s="16"/>
       <c r="O12" s="16"/>
       <c r="P12" s="16"/>
-      <c r="Q12" s="96"/>
-      <c r="R12" s="97"/>
+      <c r="Q12" s="87"/>
+      <c r="R12" s="88"/>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B13" s="64"/>
-      <c r="C13" s="90"/>
+      <c r="B13" s="77"/>
+      <c r="C13" s="97"/>
       <c r="D13" s="2" t="s">
         <v>133</v>
       </c>
@@ -3232,14 +3232,14 @@
       <c r="N13" s="32"/>
       <c r="O13" s="32"/>
       <c r="P13" s="32"/>
-      <c r="Q13" s="74"/>
-      <c r="R13" s="75"/>
+      <c r="Q13" s="67"/>
+      <c r="R13" s="68"/>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B14" s="63">
+      <c r="B14" s="76">
         <v>2</v>
       </c>
-      <c r="C14" s="63" t="s">
+      <c r="C14" s="76" t="s">
         <v>78</v>
       </c>
       <c r="D14" s="2" t="s">
@@ -3261,12 +3261,12 @@
       <c r="N14" s="32"/>
       <c r="O14" s="32"/>
       <c r="P14" s="32"/>
-      <c r="Q14" s="74"/>
-      <c r="R14" s="75"/>
+      <c r="Q14" s="67"/>
+      <c r="R14" s="68"/>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B15" s="87"/>
-      <c r="C15" s="87"/>
+      <c r="B15" s="94"/>
+      <c r="C15" s="94"/>
       <c r="D15" s="2" t="s">
         <v>100</v>
       </c>
@@ -3286,12 +3286,12 @@
       <c r="N15" s="32"/>
       <c r="O15" s="32"/>
       <c r="P15" s="32"/>
-      <c r="Q15" s="74"/>
-      <c r="R15" s="75"/>
+      <c r="Q15" s="67"/>
+      <c r="R15" s="68"/>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B16" s="87"/>
-      <c r="C16" s="87"/>
+      <c r="B16" s="94"/>
+      <c r="C16" s="94"/>
       <c r="D16" s="2" t="s">
         <v>101</v>
       </c>
@@ -3311,12 +3311,12 @@
       <c r="N16" s="32"/>
       <c r="O16" s="32"/>
       <c r="P16" s="32"/>
-      <c r="Q16" s="74"/>
-      <c r="R16" s="75"/>
+      <c r="Q16" s="67"/>
+      <c r="R16" s="68"/>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B17" s="87"/>
-      <c r="C17" s="87"/>
+      <c r="B17" s="94"/>
+      <c r="C17" s="94"/>
       <c r="D17" s="2" t="s">
         <v>103</v>
       </c>
@@ -3336,12 +3336,12 @@
       <c r="N17" s="32"/>
       <c r="O17" s="32"/>
       <c r="P17" s="32"/>
-      <c r="Q17" s="74"/>
-      <c r="R17" s="75"/>
+      <c r="Q17" s="67"/>
+      <c r="R17" s="68"/>
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B18" s="87"/>
-      <c r="C18" s="87"/>
+      <c r="B18" s="94"/>
+      <c r="C18" s="94"/>
       <c r="D18" s="2" t="s">
         <v>103</v>
       </c>
@@ -3361,12 +3361,12 @@
       <c r="N18" s="32"/>
       <c r="O18" s="32"/>
       <c r="P18" s="32"/>
-      <c r="Q18" s="74"/>
-      <c r="R18" s="75"/>
+      <c r="Q18" s="67"/>
+      <c r="R18" s="68"/>
     </row>
     <row r="19" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B19" s="64"/>
-      <c r="C19" s="64"/>
+      <c r="B19" s="77"/>
+      <c r="C19" s="77"/>
       <c r="D19" s="2" t="s">
         <v>102</v>
       </c>
@@ -3386,14 +3386,14 @@
       <c r="N19" s="32"/>
       <c r="O19" s="32"/>
       <c r="P19" s="32"/>
-      <c r="Q19" s="74"/>
-      <c r="R19" s="75"/>
+      <c r="Q19" s="67"/>
+      <c r="R19" s="68"/>
     </row>
     <row r="20" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B20" s="63">
+      <c r="B20" s="76">
         <v>3</v>
       </c>
-      <c r="C20" s="88" t="s">
+      <c r="C20" s="95" t="s">
         <v>74</v>
       </c>
       <c r="D20" s="2" t="s">
@@ -3419,14 +3419,14 @@
       <c r="N20" s="32"/>
       <c r="O20" s="32"/>
       <c r="P20" s="32"/>
-      <c r="Q20" s="74" t="s">
+      <c r="Q20" s="67" t="s">
         <v>87</v>
       </c>
-      <c r="R20" s="75"/>
+      <c r="R20" s="68"/>
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B21" s="87"/>
-      <c r="C21" s="89"/>
+      <c r="B21" s="94"/>
+      <c r="C21" s="96"/>
       <c r="D21" s="2" t="s">
         <v>110</v>
       </c>
@@ -3450,14 +3450,14 @@
       <c r="N21" s="32"/>
       <c r="O21" s="32"/>
       <c r="P21" s="32"/>
-      <c r="Q21" s="74" t="s">
+      <c r="Q21" s="67" t="s">
         <v>87</v>
       </c>
-      <c r="R21" s="75"/>
+      <c r="R21" s="68"/>
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B22" s="87"/>
-      <c r="C22" s="89"/>
+      <c r="B22" s="94"/>
+      <c r="C22" s="96"/>
       <c r="D22" s="2" t="s">
         <v>111</v>
       </c>
@@ -3477,12 +3477,12 @@
       <c r="N22" s="32"/>
       <c r="O22" s="32"/>
       <c r="P22" s="32"/>
-      <c r="Q22" s="74"/>
-      <c r="R22" s="75"/>
+      <c r="Q22" s="67"/>
+      <c r="R22" s="68"/>
     </row>
     <row r="23" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B23" s="87"/>
-      <c r="C23" s="89"/>
+      <c r="B23" s="94"/>
+      <c r="C23" s="96"/>
       <c r="D23" s="2"/>
       <c r="G23" s="21">
         <v>17</v>
@@ -3500,12 +3500,12 @@
       <c r="N23" s="32"/>
       <c r="O23" s="32"/>
       <c r="P23" s="32"/>
-      <c r="Q23" s="74"/>
-      <c r="R23" s="75"/>
+      <c r="Q23" s="67"/>
+      <c r="R23" s="68"/>
     </row>
     <row r="24" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B24" s="87"/>
-      <c r="C24" s="89"/>
+      <c r="B24" s="94"/>
+      <c r="C24" s="96"/>
       <c r="D24" s="2"/>
       <c r="G24" s="21">
         <v>18</v>
@@ -3523,12 +3523,12 @@
       <c r="N24" s="32"/>
       <c r="O24" s="32"/>
       <c r="P24" s="32"/>
-      <c r="Q24" s="74"/>
-      <c r="R24" s="75"/>
+      <c r="Q24" s="67"/>
+      <c r="R24" s="68"/>
     </row>
     <row r="25" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B25" s="64"/>
-      <c r="C25" s="90"/>
+      <c r="B25" s="77"/>
+      <c r="C25" s="97"/>
       <c r="D25" s="2"/>
       <c r="G25" s="21">
         <v>19</v>
@@ -3550,10 +3550,10 @@
       <c r="R25" s="2"/>
     </row>
     <row r="26" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B26" s="63">
+      <c r="B26" s="76">
         <v>4</v>
       </c>
-      <c r="C26" s="88" t="s">
+      <c r="C26" s="95" t="s">
         <v>120</v>
       </c>
       <c r="D26" s="2" t="s">
@@ -3579,8 +3579,8 @@
       <c r="R26" s="2"/>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B27" s="87"/>
-      <c r="C27" s="89"/>
+      <c r="B27" s="94"/>
+      <c r="C27" s="96"/>
       <c r="D27" s="2" t="s">
         <v>129</v>
       </c>
@@ -3602,13 +3602,13 @@
       <c r="R27" s="2"/>
     </row>
     <row r="28" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B28" s="87"/>
-      <c r="C28" s="89"/>
+      <c r="B28" s="94"/>
+      <c r="C28" s="96"/>
       <c r="D28" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="G28" s="84"/>
-      <c r="H28" s="84"/>
+      <c r="G28" s="62"/>
+      <c r="H28" s="62"/>
       <c r="I28" s="92"/>
       <c r="J28" s="92"/>
       <c r="K28" s="92"/>
@@ -3617,41 +3617,50 @@
       <c r="N28" s="41"/>
     </row>
     <row r="29" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B29" s="87"/>
-      <c r="C29" s="89"/>
+      <c r="B29" s="94"/>
+      <c r="C29" s="96"/>
       <c r="D29" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="I29" s="91"/>
-      <c r="J29" s="91"/>
-      <c r="K29" s="91"/>
-      <c r="L29" s="91"/>
-      <c r="M29" s="91"/>
+      <c r="I29" s="98"/>
+      <c r="J29" s="98"/>
+      <c r="K29" s="98"/>
+      <c r="L29" s="98"/>
+      <c r="M29" s="98"/>
       <c r="N29" s="42"/>
     </row>
     <row r="30" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B30" s="87"/>
-      <c r="C30" s="89"/>
+      <c r="B30" s="94"/>
+      <c r="C30" s="96"/>
       <c r="D30" s="2" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="31" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B31" s="64"/>
-      <c r="C31" s="90"/>
+      <c r="B31" s="77"/>
+      <c r="C31" s="97"/>
       <c r="D31" s="2" t="s">
         <v>97</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="Q19:R19"/>
-    <mergeCell ref="Q20:R20"/>
-    <mergeCell ref="Q12:R12"/>
-    <mergeCell ref="K5:P5"/>
-    <mergeCell ref="Q9:R9"/>
-    <mergeCell ref="Q10:R10"/>
-    <mergeCell ref="Q11:R11"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="B26:B31"/>
+    <mergeCell ref="C26:C31"/>
+    <mergeCell ref="B8:B13"/>
+    <mergeCell ref="C8:C13"/>
+    <mergeCell ref="B14:B19"/>
+    <mergeCell ref="C14:C19"/>
+    <mergeCell ref="C20:C25"/>
+    <mergeCell ref="B20:B25"/>
+    <mergeCell ref="I29:M29"/>
+    <mergeCell ref="G4:R4"/>
+    <mergeCell ref="Q6:R6"/>
+    <mergeCell ref="G28:H28"/>
     <mergeCell ref="I28:M28"/>
     <mergeCell ref="B6:D6"/>
     <mergeCell ref="Q5:R5"/>
@@ -3668,22 +3677,13 @@
     <mergeCell ref="Q7:R7"/>
     <mergeCell ref="Q8:R8"/>
     <mergeCell ref="Q18:R18"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="B26:B31"/>
-    <mergeCell ref="C26:C31"/>
-    <mergeCell ref="B8:B13"/>
-    <mergeCell ref="C8:C13"/>
-    <mergeCell ref="B14:B19"/>
-    <mergeCell ref="C14:C19"/>
-    <mergeCell ref="C20:C25"/>
-    <mergeCell ref="B20:B25"/>
-    <mergeCell ref="I29:M29"/>
-    <mergeCell ref="G4:R4"/>
-    <mergeCell ref="Q6:R6"/>
-    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="Q19:R19"/>
+    <mergeCell ref="Q20:R20"/>
+    <mergeCell ref="Q12:R12"/>
+    <mergeCell ref="K5:P5"/>
+    <mergeCell ref="Q9:R9"/>
+    <mergeCell ref="Q10:R10"/>
+    <mergeCell ref="Q11:R11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3698,8 +3698,8 @@
   </sheetPr>
   <dimension ref="B1:P21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="72" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="72" workbookViewId="0">
+      <selection activeCell="S12" sqref="S12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3723,54 +3723,54 @@
       <c r="E1" s="60"/>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B3" s="114" t="s">
+      <c r="B3" s="137" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="114"/>
-      <c r="D3" s="114"/>
-      <c r="E3" s="114"/>
-      <c r="F3" s="114"/>
-      <c r="G3" s="114"/>
-      <c r="H3" s="114"/>
-      <c r="I3" s="114"/>
-      <c r="J3" s="114"/>
-      <c r="K3" s="114"/>
-      <c r="L3" s="114"/>
-      <c r="M3" s="114"/>
-      <c r="N3" s="114"/>
+      <c r="C3" s="137"/>
+      <c r="D3" s="137"/>
+      <c r="E3" s="137"/>
+      <c r="F3" s="137"/>
+      <c r="G3" s="137"/>
+      <c r="H3" s="137"/>
+      <c r="I3" s="137"/>
+      <c r="J3" s="137"/>
+      <c r="K3" s="137"/>
+      <c r="L3" s="137"/>
+      <c r="M3" s="137"/>
+      <c r="N3" s="137"/>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B4" s="70" t="s">
+      <c r="B4" s="83" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="106" t="s">
+      <c r="C4" s="129" t="s">
         <v>43</v>
       </c>
-      <c r="D4" s="119" t="s">
+      <c r="D4" s="111" t="s">
         <v>44</v>
       </c>
-      <c r="E4" s="80" t="s">
+      <c r="E4" s="71" t="s">
         <v>45</v>
       </c>
-      <c r="F4" s="78" t="s">
+      <c r="F4" s="69" t="s">
         <v>27</v>
       </c>
-      <c r="G4" s="83"/>
-      <c r="H4" s="83"/>
-      <c r="I4" s="83"/>
-      <c r="J4" s="83"/>
-      <c r="K4" s="83"/>
-      <c r="L4" s="79"/>
-      <c r="M4" s="82" t="s">
+      <c r="G4" s="74"/>
+      <c r="H4" s="74"/>
+      <c r="I4" s="74"/>
+      <c r="J4" s="74"/>
+      <c r="K4" s="74"/>
+      <c r="L4" s="70"/>
+      <c r="M4" s="73" t="s">
         <v>28</v>
       </c>
-      <c r="N4" s="82"/>
+      <c r="N4" s="73"/>
     </row>
     <row r="5" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="118"/>
-      <c r="C5" s="107"/>
-      <c r="D5" s="120"/>
-      <c r="E5" s="105"/>
+      <c r="B5" s="110"/>
+      <c r="C5" s="130"/>
+      <c r="D5" s="112"/>
+      <c r="E5" s="128"/>
       <c r="F5" s="21" t="s">
         <v>83</v>
       </c>
@@ -3782,8 +3782,8 @@
       </c>
       <c r="I5" s="24"/>
       <c r="J5" s="24"/>
-      <c r="K5" s="101"/>
-      <c r="L5" s="102"/>
+      <c r="K5" s="124"/>
+      <c r="L5" s="125"/>
       <c r="M5" s="24" t="s">
         <v>29</v>
       </c>
@@ -3795,7 +3795,7 @@
       <c r="B6" s="22">
         <v>1</v>
       </c>
-      <c r="C6" s="116" t="s">
+      <c r="C6" s="108" t="s">
         <v>47</v>
       </c>
       <c r="D6" s="28" t="s">
@@ -3815,8 +3815,8 @@
       </c>
       <c r="I6" s="27"/>
       <c r="J6" s="27"/>
-      <c r="K6" s="103"/>
-      <c r="L6" s="104"/>
+      <c r="K6" s="126"/>
+      <c r="L6" s="127"/>
       <c r="M6" s="27" t="s">
         <v>87</v>
       </c>
@@ -3829,7 +3829,7 @@
         <f>B6+1</f>
         <v>2</v>
       </c>
-      <c r="C7" s="116"/>
+      <c r="C7" s="108"/>
       <c r="D7" s="29" t="s">
         <v>49</v>
       </c>
@@ -3847,8 +3847,8 @@
       </c>
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
-      <c r="K7" s="108"/>
-      <c r="L7" s="109"/>
+      <c r="K7" s="131"/>
+      <c r="L7" s="132"/>
       <c r="M7" s="8" t="s">
         <v>88</v>
       </c>
@@ -3861,7 +3861,7 @@
         <f t="shared" ref="B8:B13" si="0">B7+1</f>
         <v>3</v>
       </c>
-      <c r="C8" s="116"/>
+      <c r="C8" s="108"/>
       <c r="D8" s="29" t="s">
         <v>50</v>
       </c>
@@ -3893,7 +3893,7 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C9" s="116"/>
+      <c r="C9" s="108"/>
       <c r="D9" s="29" t="s">
         <v>107</v>
       </c>
@@ -3911,8 +3911,8 @@
       </c>
       <c r="I9" s="10"/>
       <c r="J9" s="10"/>
-      <c r="K9" s="110"/>
-      <c r="L9" s="111"/>
+      <c r="K9" s="133"/>
+      <c r="L9" s="134"/>
       <c r="M9" s="10" t="s">
         <v>88</v>
       </c>
@@ -3925,7 +3925,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C10" s="116"/>
+      <c r="C10" s="108"/>
       <c r="D10" s="29" t="s">
         <v>31</v>
       </c>
@@ -3944,10 +3944,10 @@
       <c r="I10" s="32"/>
       <c r="J10" s="32"/>
       <c r="K10" s="32"/>
-      <c r="L10" s="74" t="s">
+      <c r="L10" s="67" t="s">
         <v>87</v>
       </c>
-      <c r="M10" s="75"/>
+      <c r="M10" s="68"/>
       <c r="N10" s="56" t="s">
         <v>87</v>
       </c>
@@ -3957,7 +3957,7 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C11" s="116"/>
+      <c r="C11" s="108"/>
       <c r="D11" s="29" t="s">
         <v>31</v>
       </c>
@@ -3976,10 +3976,10 @@
       <c r="I11" s="32"/>
       <c r="J11" s="32"/>
       <c r="K11" s="32"/>
-      <c r="L11" s="74" t="s">
+      <c r="L11" s="67" t="s">
         <v>87</v>
       </c>
-      <c r="M11" s="75"/>
+      <c r="M11" s="68"/>
       <c r="N11" s="56" t="s">
         <v>87</v>
       </c>
@@ -3989,7 +3989,7 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C12" s="116"/>
+      <c r="C12" s="108"/>
       <c r="D12" s="29"/>
       <c r="E12" s="10" t="s">
         <v>136</v>
@@ -4005,8 +4005,8 @@
       </c>
       <c r="I12" s="9"/>
       <c r="J12" s="9"/>
-      <c r="K12" s="112"/>
-      <c r="L12" s="113"/>
+      <c r="K12" s="135"/>
+      <c r="L12" s="136"/>
       <c r="M12" s="5" t="s">
         <v>87</v>
       </c>
@@ -4019,7 +4019,7 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C13" s="117"/>
+      <c r="C13" s="109"/>
       <c r="D13" s="30"/>
       <c r="E13" s="23" t="s">
         <v>137</v>
@@ -4035,8 +4035,8 @@
       </c>
       <c r="I13" s="23"/>
       <c r="J13" s="23"/>
-      <c r="K13" s="99"/>
-      <c r="L13" s="100"/>
+      <c r="K13" s="122"/>
+      <c r="L13" s="123"/>
       <c r="M13" s="23" t="s">
         <v>88</v>
       </c>
@@ -4071,98 +4071,98 @@
       <c r="H15" s="7"/>
       <c r="I15" s="7"/>
       <c r="J15" s="7"/>
-      <c r="K15" s="115"/>
-      <c r="L15" s="115"/>
+      <c r="K15" s="107"/>
+      <c r="L15" s="107"/>
       <c r="M15" s="7"/>
     </row>
     <row r="16" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="M16" s="7"/>
     </row>
     <row r="17" spans="2:16" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="C17" s="127" t="s">
+      <c r="C17" s="101" t="s">
         <v>52</v>
       </c>
-      <c r="D17" s="128"/>
-      <c r="E17" s="128"/>
-      <c r="F17" s="129"/>
+      <c r="D17" s="103"/>
+      <c r="E17" s="103"/>
+      <c r="F17" s="104"/>
       <c r="G17" s="37" t="s">
         <v>53</v>
       </c>
-      <c r="H17" s="127" t="s">
+      <c r="H17" s="101" t="s">
         <v>54</v>
       </c>
-      <c r="I17" s="130"/>
-      <c r="J17" s="128"/>
-      <c r="K17" s="128"/>
-      <c r="L17" s="129"/>
-      <c r="M17" s="127" t="s">
+      <c r="I17" s="102"/>
+      <c r="J17" s="103"/>
+      <c r="K17" s="103"/>
+      <c r="L17" s="104"/>
+      <c r="M17" s="101" t="s">
         <v>55</v>
       </c>
-      <c r="N17" s="130"/>
-      <c r="O17" s="128"/>
-      <c r="P17" s="129"/>
+      <c r="N17" s="102"/>
+      <c r="O17" s="103"/>
+      <c r="P17" s="104"/>
     </row>
     <row r="18" spans="2:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="123" t="s">
+      <c r="B18" s="115" t="s">
         <v>43</v>
       </c>
-      <c r="C18" s="124" t="s">
+      <c r="C18" s="116" t="s">
         <v>56</v>
       </c>
-      <c r="D18" s="125" t="s">
+      <c r="D18" s="100" t="s">
         <v>57</v>
       </c>
-      <c r="E18" s="125" t="s">
+      <c r="E18" s="100" t="s">
         <v>58</v>
       </c>
-      <c r="F18" s="126" t="s">
+      <c r="F18" s="99" t="s">
         <v>59</v>
       </c>
-      <c r="G18" s="135" t="s">
+      <c r="G18" s="121" t="s">
         <v>60</v>
       </c>
-      <c r="H18" s="131" t="s">
+      <c r="H18" s="117" t="s">
         <v>61</v>
       </c>
-      <c r="I18" s="132"/>
-      <c r="J18" s="125" t="s">
+      <c r="I18" s="118"/>
+      <c r="J18" s="100" t="s">
         <v>56</v>
       </c>
-      <c r="K18" s="125" t="s">
+      <c r="K18" s="100" t="s">
         <v>57</v>
       </c>
-      <c r="L18" s="126" t="s">
+      <c r="L18" s="99" t="s">
         <v>58</v>
       </c>
-      <c r="M18" s="136" t="s">
+      <c r="M18" s="105" t="s">
         <v>61</v>
       </c>
-      <c r="N18" s="125" t="s">
+      <c r="N18" s="100" t="s">
         <v>56</v>
       </c>
-      <c r="O18" s="125" t="s">
+      <c r="O18" s="100" t="s">
         <v>57</v>
       </c>
-      <c r="P18" s="126" t="s">
+      <c r="P18" s="99" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B19" s="123"/>
-      <c r="C19" s="124"/>
-      <c r="D19" s="125"/>
-      <c r="E19" s="125"/>
-      <c r="F19" s="126"/>
-      <c r="G19" s="135"/>
-      <c r="H19" s="133"/>
-      <c r="I19" s="134"/>
-      <c r="J19" s="125"/>
-      <c r="K19" s="125"/>
-      <c r="L19" s="126"/>
-      <c r="M19" s="137"/>
-      <c r="N19" s="125"/>
-      <c r="O19" s="125"/>
-      <c r="P19" s="126"/>
+      <c r="B19" s="115"/>
+      <c r="C19" s="116"/>
+      <c r="D19" s="100"/>
+      <c r="E19" s="100"/>
+      <c r="F19" s="99"/>
+      <c r="G19" s="121"/>
+      <c r="H19" s="119"/>
+      <c r="I19" s="120"/>
+      <c r="J19" s="100"/>
+      <c r="K19" s="100"/>
+      <c r="L19" s="99"/>
+      <c r="M19" s="106"/>
+      <c r="N19" s="100"/>
+      <c r="O19" s="100"/>
+      <c r="P19" s="99"/>
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B20" s="40" t="s">
@@ -4181,10 +4181,10 @@
         <v>0</v>
       </c>
       <c r="G20" s="44"/>
-      <c r="H20" s="121" t="s">
+      <c r="H20" s="113" t="s">
         <v>115</v>
       </c>
-      <c r="I20" s="122"/>
+      <c r="I20" s="114"/>
       <c r="J20" s="2">
         <v>0</v>
       </c>
@@ -4212,12 +4212,20 @@
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="L18:L19"/>
-    <mergeCell ref="O18:O19"/>
-    <mergeCell ref="P18:P19"/>
-    <mergeCell ref="M17:P17"/>
-    <mergeCell ref="M18:M19"/>
-    <mergeCell ref="N18:N19"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="F4:L4"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="B3:N3"/>
+    <mergeCell ref="L10:M10"/>
     <mergeCell ref="K15:L15"/>
     <mergeCell ref="C6:C13"/>
     <mergeCell ref="B4:B5"/>
@@ -4234,20 +4242,12 @@
     <mergeCell ref="H18:I19"/>
     <mergeCell ref="G18:G19"/>
     <mergeCell ref="K18:K19"/>
-    <mergeCell ref="L11:M11"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="F4:L4"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="B3:N3"/>
-    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="L18:L19"/>
+    <mergeCell ref="O18:O19"/>
+    <mergeCell ref="P18:P19"/>
+    <mergeCell ref="M17:P17"/>
+    <mergeCell ref="M18:M19"/>
+    <mergeCell ref="N18:N19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4256,6 +4256,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010058284A30843C9F43BD758DDD8294D484" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6d50638930d08c51b5585735b2be047e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="fed1744a-f275-4023-9290-77fd546fd730" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4acb07121b76573bb3c966f3dcb1b903" ns2:_="">
     <xsd:import namespace="fed1744a-f275-4023-9290-77fd546fd730"/>
@@ -4399,22 +4414,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF0EB622-FDCF-4321-9FF5-C0B282D1670E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2BC1EB47-4FFF-47F3-894F-DED91590EA19}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33EFF49E-866D-4BFD-B7FD-9BB436667B53}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4430,21 +4447,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2BC1EB47-4FFF-47F3-894F-DED91590EA19}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF0EB622-FDCF-4321-9FF5-C0B282D1670E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>